<commit_message>
Versión final editora CS_10_01
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion01/Solicitud grafica_CS_10_01_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion01/Solicitud grafica_CS_10_01_CO.xlsx
@@ -609,9 +609,6 @@
     <t>Firma del final de la Guerra Fría por parte de Gorbachov y Reagan.</t>
   </si>
   <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
     <t>CS_10_01_CO_IMG04</t>
   </si>
   <si>
@@ -821,6 +818,9 @@
   </si>
   <si>
     <t>Mapa de la Unión Europea.</t>
+  </si>
+  <si>
+    <t>http://upload.wikimedia.org/wikipedia/commons/d/d2/Yalta_summit_1945_with_Churchill,_Roosevelt,_Stalin.jpg (Churchil, Stalin, Roosevalt, protagonistas de la Segunda Guerra Mundial y de la Guerra fría); http://img.desmotivaciones.es/201301/FidelyelCheinedita.jpg (Castro y el Che, figuras de la Guerra Fría en América Latina); http://upload.wikimedia.org/wikipedia/commons/7/7e/John_Kennedy,_Nikita_Khrushchev_1961.jpg (John Kennedy, Nikita Khrushchev)</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1011,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1055,6 +1055,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1785,6 +1791,14 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1870,16 +1884,8 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -2728,9 +2734,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.5"/>
@@ -2768,14 +2774,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="F2" s="82" t="s">
+      <c r="D2" s="94"/>
+      <c r="F2" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="83"/>
+      <c r="G2" s="87"/>
       <c r="H2" s="50"/>
       <c r="I2" s="50"/>
       <c r="J2" s="15"/>
@@ -2785,14 +2791,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="91">
+      <c r="C3" s="95">
         <v>10</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="F3" s="84">
+      <c r="D3" s="96"/>
+      <c r="F3" s="88">
         <v>42069</v>
       </c>
-      <c r="G3" s="85"/>
+      <c r="G3" s="89"/>
       <c r="H3" s="50"/>
       <c r="I3" s="50"/>
       <c r="J3" s="15"/>
@@ -2802,10 +2808,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="97" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="96"/>
       <c r="E4" s="5"/>
       <c r="F4" s="49" t="s">
         <v>55</v>
@@ -2821,10 +2827,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="94" t="s">
+      <c r="C5" s="98" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="95"/>
+      <c r="D5" s="99"/>
       <c r="E5" s="5"/>
       <c r="F5" s="47" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2873,12 +2879,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="87"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="88"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="92"/>
       <c r="J8" s="17"/>
       <c r="K8" s="11"/>
       <c r="L8" s="2"/>
@@ -2998,7 +3004,7 @@
       <c r="A12" s="75" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="82" t="s">
         <v>176</v>
       </c>
       <c r="C12" s="77" t="s">
@@ -3030,12 +3036,12 @@
       </c>
       <c r="K12" s="18"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="15.75">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="243">
       <c r="A13" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="115" t="s">
-        <v>178</v>
+      <c r="B13" s="118" t="s">
+        <v>241</v>
       </c>
       <c r="C13" s="77" t="s">
         <v>103</v>
@@ -3047,7 +3053,7 @@
         <v>167</v>
       </c>
       <c r="F13" s="79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G13" s="13" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3062,7 +3068,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="80" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K13" s="18"/>
     </row>
@@ -3083,7 +3089,7 @@
         <v>167</v>
       </c>
       <c r="F14" s="79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G14" s="13" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3098,7 +3104,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="80" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K14" s="18"/>
     </row>
@@ -3107,7 +3113,7 @@
         <v>153</v>
       </c>
       <c r="B15" s="81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C15" s="77" t="s">
         <v>103</v>
@@ -3119,7 +3125,7 @@
         <v>167</v>
       </c>
       <c r="F15" s="79" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G15" s="13" t="str">
         <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3134,7 +3140,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="80" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K15" s="20"/>
     </row>
@@ -3143,7 +3149,7 @@
         <v>154</v>
       </c>
       <c r="B16" s="81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C16" s="77" t="s">
         <v>103</v>
@@ -3155,7 +3161,7 @@
         <v>167</v>
       </c>
       <c r="F16" s="79" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G16" s="13" t="str">
         <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3170,7 +3176,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="80" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K16" s="31"/>
     </row>
@@ -3179,7 +3185,7 @@
         <v>155</v>
       </c>
       <c r="B17" s="81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C17" s="77" t="s">
         <v>103</v>
@@ -3191,7 +3197,7 @@
         <v>167</v>
       </c>
       <c r="F17" s="79" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="13" t="str">
         <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3206,7 +3212,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="80" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K17" s="20"/>
     </row>
@@ -3215,7 +3221,7 @@
         <v>156</v>
       </c>
       <c r="B18" s="81" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C18" s="77" t="s">
         <v>103</v>
@@ -3227,7 +3233,7 @@
         <v>167</v>
       </c>
       <c r="F18" s="79" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G18" s="13" t="str">
         <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3242,7 +3248,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J18" s="80" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K18" s="20"/>
     </row>
@@ -3251,7 +3257,7 @@
         <v>157</v>
       </c>
       <c r="B19" s="81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C19" s="77" t="s">
         <v>103</v>
@@ -3263,7 +3269,7 @@
         <v>167</v>
       </c>
       <c r="F19" s="79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G19" s="13" t="str">
         <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3278,7 +3284,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="80" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K19" s="31"/>
     </row>
@@ -3287,7 +3293,7 @@
         <v>158</v>
       </c>
       <c r="B20" s="81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C20" s="77" t="s">
         <v>103</v>
@@ -3299,7 +3305,7 @@
         <v>167</v>
       </c>
       <c r="F20" s="79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G20" s="13" t="str">
         <f>IF(F20&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3314,7 +3320,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="80" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K20" s="20"/>
     </row>
@@ -3322,8 +3328,8 @@
       <c r="A21" s="75" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="116" t="s">
-        <v>201</v>
+      <c r="B21" s="83" t="s">
+        <v>200</v>
       </c>
       <c r="C21" s="77" t="s">
         <v>103</v>
@@ -3335,7 +3341,7 @@
         <v>167</v>
       </c>
       <c r="F21" s="79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G21" s="13" t="str">
         <f>IF(F21&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3350,7 +3356,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J21" s="80" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K21" s="20"/>
     </row>
@@ -3359,7 +3365,7 @@
         <v>98</v>
       </c>
       <c r="B22" s="81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="77" t="s">
         <v>103</v>
@@ -3371,7 +3377,7 @@
         <v>167</v>
       </c>
       <c r="F22" s="79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G22" s="13" t="str">
         <f>IF(F22&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3386,7 +3392,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="80" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K22" s="19"/>
     </row>
@@ -3395,7 +3401,7 @@
         <v>160</v>
       </c>
       <c r="B23" s="81" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C23" s="77" t="s">
         <v>103</v>
@@ -3407,7 +3413,7 @@
         <v>167</v>
       </c>
       <c r="F23" s="79" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G23" s="13" t="str">
         <f>IF(F23&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3422,7 +3428,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K23" s="18"/>
     </row>
@@ -3431,7 +3437,7 @@
         <v>161</v>
       </c>
       <c r="B24" s="81" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C24" s="77" t="s">
         <v>103</v>
@@ -3443,7 +3449,7 @@
         <v>167</v>
       </c>
       <c r="F24" s="79" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G24" s="13" t="str">
         <f>IF(F24&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3458,7 +3464,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J24" s="80" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K24" s="14"/>
     </row>
@@ -3467,7 +3473,7 @@
         <v>162</v>
       </c>
       <c r="B25" s="81" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C25" s="77" t="s">
         <v>103</v>
@@ -3479,7 +3485,7 @@
         <v>167</v>
       </c>
       <c r="F25" s="79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G25" s="13" t="str">
         <f>IF(F25&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3494,7 +3500,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K25" s="18"/>
     </row>
@@ -3503,7 +3509,7 @@
         <v>163</v>
       </c>
       <c r="B26" s="81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C26" s="77" t="s">
         <v>103</v>
@@ -3515,7 +3521,7 @@
         <v>167</v>
       </c>
       <c r="F26" s="79" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G26" s="13" t="str">
         <f>IF(F26&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3530,7 +3536,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="80" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K26" s="18"/>
     </row>
@@ -3539,7 +3545,7 @@
         <v>164</v>
       </c>
       <c r="B27" s="81" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C27" s="77" t="s">
         <v>103</v>
@@ -3551,7 +3557,7 @@
         <v>167</v>
       </c>
       <c r="F27" s="79" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G27" s="13" t="str">
         <f>IF(F27&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3566,7 +3572,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J27" s="80" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K27" s="18"/>
     </row>
@@ -3575,7 +3581,7 @@
         <v>165</v>
       </c>
       <c r="B28" s="81" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" s="77" t="s">
         <v>103</v>
@@ -3587,7 +3593,7 @@
         <v>167</v>
       </c>
       <c r="F28" s="79" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G28" s="13" t="str">
         <f>IF(F28&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3602,16 +3608,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J28" s="80" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K28" s="18"/>
     </row>
     <row r="29" spans="1:11" s="11" customFormat="1" ht="15.75">
       <c r="A29" s="75" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B29" s="81" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C29" s="77" t="s">
         <v>103</v>
@@ -3623,7 +3629,7 @@
         <v>167</v>
       </c>
       <c r="F29" s="79" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G29" s="13" t="str">
         <f>IF(F29&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3638,16 +3644,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J29" s="80" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K29" s="18"/>
     </row>
     <row r="30" spans="1:11" s="11" customFormat="1" ht="16.5" thickBot="1">
       <c r="A30" s="75" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B30" s="81" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C30" s="77" t="s">
         <v>103</v>
@@ -3659,7 +3665,7 @@
         <v>167</v>
       </c>
       <c r="F30" s="79" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G30" s="13" t="str">
         <f>IF(F30&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3674,16 +3680,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J30" s="80" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K30" s="18"/>
     </row>
     <row r="31" spans="1:11" s="11" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
       <c r="A31" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="B31" s="117" t="s">
-        <v>237</v>
+        <v>224</v>
+      </c>
+      <c r="B31" s="84" t="s">
+        <v>236</v>
       </c>
       <c r="C31" s="77" t="s">
         <v>103</v>
@@ -3694,8 +3700,8 @@
       <c r="E31" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="F31" s="118" t="s">
-        <v>238</v>
+      <c r="F31" s="85" t="s">
+        <v>237</v>
       </c>
       <c r="G31" s="13" t="str">
         <f>IF(F31&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3710,13 +3716,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J31" s="80" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K31" s="18"/>
     </row>
     <row r="32" spans="1:11" s="11" customFormat="1" ht="15.75">
       <c r="A32" s="75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B32" s="81" t="s">
         <v>171</v>
@@ -3731,7 +3737,7 @@
         <v>167</v>
       </c>
       <c r="F32" s="79" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G32" s="13" t="str">
         <f>IF(F32&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -3746,7 +3752,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J32" s="80" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K32" s="18"/>
     </row>
@@ -3928,14 +3934,14 @@
     </row>
     <row r="41" spans="1:11" s="11" customFormat="1">
       <c r="A41" s="75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B41" s="26"/>
       <c r="C41" s="26"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13" t="str">
-        <f t="shared" ref="F11:F74" si="1">IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE($C$7,"_",$A41,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I41="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F41:F74" si="1">IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE($C$7,"_",$A41,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I41="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G41" s="13" t="str">
@@ -3955,7 +3961,7 @@
     </row>
     <row r="42" spans="1:11" s="11" customFormat="1">
       <c r="A42" s="75" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="26"/>
@@ -5714,25 +5720,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="100"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+      <c r="F1" s="104"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="41"/>
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="102"/>
-      <c r="E2" s="103"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
       <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -5740,11 +5746,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="41"/>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="E3" s="109"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="113"/>
       <c r="F3" s="42"/>
       <c r="H3" s="32" t="s">
         <v>18</v>
@@ -5795,11 +5801,11 @@
       <c r="C5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="110" t="str">
+      <c r="D5" s="114" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="111"/>
+      <c r="E5" s="115"/>
       <c r="F5" s="42"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
@@ -5844,12 +5850,12 @@
       <c r="C7" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="96" t="str">
+      <c r="D7" s="100" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="96"/>
-      <c r="F7" s="97"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="101"/>
       <c r="H7" s="32" t="s">
         <v>24</v>
       </c>
@@ -5943,14 +5949,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="99"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="100"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="103"/>
+      <c r="F13" s="104"/>
       <c r="I13" s="32" t="s">
         <v>33</v>
       </c>
@@ -5983,12 +5989,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="41"/>
-      <c r="C15" s="101" t="s">
+      <c r="C15" s="105" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="103"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="107"/>
       <c r="J15" s="32">
         <v>12</v>
       </c>
@@ -6028,12 +6034,12 @@
       <c r="C17" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="104" t="str">
+      <c r="D17" s="108" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="105"/>
-      <c r="F17" s="106"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="110"/>
       <c r="J17" s="32">
         <v>14</v>
       </c>
@@ -6049,12 +6055,12 @@
       <c r="C18" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="96" t="str">
+      <c r="D18" s="100" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="97"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="101"/>
       <c r="J18" s="32">
         <v>15</v>
       </c>
@@ -6446,41 +6452,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="116" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="112" t="s">
+      <c r="E1" s="116" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="112" t="s">
+      <c r="F1" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="112" t="s">
+      <c r="G1" s="116" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="113" t="s">
+      <c r="H1" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="112"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
+      <c r="A2" s="116"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
       <c r="H2" s="51" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
Mabel Lara: segunda edición
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion01/Solicitud grafica_CS_10_01_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion01/Solicitud grafica_CS_10_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zambanitos\Documents\MABEL\TRABAJO\PLANETA\JOSE_GUILLERMO\UNIDAD1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zambanitos\Documents\GitHub\CienciasSociales\fuentes\contenidos\grado10\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="273">
   <si>
     <t>Fecha:</t>
   </si>
@@ -612,20 +612,6 @@
     <t>CS_10_01_CO_IMG04</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Galería de fotos de los siguientes políticos: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Churchil, Stalin, Roosevalt, Marshall, Fidel Castro, Che Guevara, Kennedy, Nikita Krushev</t>
-    </r>
-  </si>
-  <si>
     <t>CS_10_01_CO_IMG05</t>
   </si>
   <si>
@@ -820,7 +806,114 @@
     <t>Mapa de la Unión Europea.</t>
   </si>
   <si>
-    <t>http://upload.wikimedia.org/wikipedia/commons/d/d2/Yalta_summit_1945_with_Churchill,_Roosevelt,_Stalin.jpg (Churchil, Stalin, Roosevalt, protagonistas de la Segunda Guerra Mundial y de la Guerra fría); http://img.desmotivaciones.es/201301/FidelyelCheinedita.jpg (Castro y el Che, figuras de la Guerra Fría en América Latina); http://upload.wikimedia.org/wikipedia/commons/7/7e/John_Kennedy,_Nikita_Khrushchev_1961.jpg (John Kennedy, Nikita Khrushchev)</t>
+    <t>F24</t>
+  </si>
+  <si>
+    <t>F25</t>
+  </si>
+  <si>
+    <t>F26</t>
+  </si>
+  <si>
+    <t>F27</t>
+  </si>
+  <si>
+    <t>F28</t>
+  </si>
+  <si>
+    <t>F29</t>
+  </si>
+  <si>
+    <t>F30</t>
+  </si>
+  <si>
+    <t>F31</t>
+  </si>
+  <si>
+    <t>F34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://upload.wikimedia.org/wikipedia/commons/d/d2/Yalta_summit_1945_with_Churchill,_Roosevelt,_Stalin.jpg (Churchil, Stalin, Roosevalt, protagonistas de la Segunda Guerra Mundial y de la Guerra fría); </t>
+  </si>
+  <si>
+    <t>http://img.desmotivaciones.es/201301/FidelyelCheinedita.jpg (Castro y el Che, figuras de la Guerra Fría en América Latina); http://upload.wikimedia.org/wikipedia/commons/7/7e/John_Kennedy,_Nikita_Khrushchev_1961.jpg (John Kennedy, Nikita Khrushchev)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Galería de fotos de los siguientes políticos: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Churchil, Stalin, Roosevalt, Marshall, </t>
+    </r>
+  </si>
+  <si>
+    <t>Fidel Castro, Che Guevara, Kennedy, Nikita Krushev</t>
+  </si>
+  <si>
+    <t>http://www.shutterstock.com/cat.mhtml?searchterm=cortina%20de%20hierro&amp;autocomplete_id=142972510085113220000&amp;language=es&amp;lang=es&amp;search_source=&amp;safesearch=1&amp;version=llv1&amp;media_type=&amp;page=1&amp;inline=237232840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fotografía de control policial </t>
+  </si>
+  <si>
+    <t>http://www.shutterstock.com/cat.mhtml?lang=es&amp;language=es&amp;ref_site=photo&amp;search_source=search_form&amp;version=llv1&amp;anyorall=all&amp;safesearch=1&amp;use_local_boost=1&amp;search_tracking_id=sz0Q8cVoN1MZLDqeQFqTpA&amp;searchterm=URSS&amp;show_color_wheel=1&amp;orient=&amp;commercial_ok=&amp;media_type=images&amp;search_cat=&amp;searchtermx=&amp;photographer_name=&amp;people_gender=&amp;people_age=&amp;people_ethnicity=&amp;people_number=&amp;color=&amp;page=1&amp;inline=218932498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fotografía turística de la URSS </t>
+  </si>
+  <si>
+    <t>http://thumb7.shutterstock.com/display_pic_with_logo/5914/5914,1119356335,1/stock-photo-romanian-communist-peasants-working-on-field-383261.jpg</t>
+  </si>
+  <si>
+    <t>Campesinos en la urss</t>
+  </si>
+  <si>
+    <t>http://thumb101.shutterstock.com/display_pic_with_logo/5225/166423973/stock-photo-petrozavodsk-russia-may-members-of-the-communist-party-rally-near-the-monument-to-lenin-by-166423973.jpg</t>
+  </si>
+  <si>
+    <t>Miembros del partido comunista soviético</t>
+  </si>
+  <si>
+    <t>http://thumb9.shutterstock.com/display_pic_with_logo/2864470/254323222/stock-photo-lenin-monument-in-kharkov-which-was-demolished-in-under-the-bright-winter-sky-until-it-254323222.jpg</t>
+  </si>
+  <si>
+    <t>Monumento de Lenin</t>
+  </si>
+  <si>
+    <t>http://thumb1.shutterstock.com/display_pic_with_logo/51142/51142,1178608277,4/stock-photo-old-rocket-installation-in-a-museum-of-arms-3251682.jpg</t>
+  </si>
+  <si>
+    <t>Misiles nucleares</t>
+  </si>
+  <si>
+    <t>http://thumb1.shutterstock.com/display_pic_with_logo/117589/141337504/stock-photo-oil-and-gas-industry-work-of-oil-pump-jack-on-a-oil-field-winter-extraction-of-oil-oil-industry-141337504.jpg</t>
+  </si>
+  <si>
+    <t>Pozo petrolero en Rusia</t>
+  </si>
+  <si>
+    <t>http://thumb7.shutterstock.com/display_pic_with_logo/434719/198363935/stock-photo-berlin-germany-june-people-watching-to-berlin-wall-on-june-berlin-germany-198363935.jpg</t>
+  </si>
+  <si>
+    <t>Muro de Berlín</t>
+  </si>
+  <si>
+    <t>Imagen de la Franja de Gaza</t>
+  </si>
+  <si>
+    <t>http://thumb7.shutterstock.com/display_pic_with_logo/1288117/204436981/stock-photo--jewish-conflicts-in-jerusalem-rock-dome-on-the-temple-mount-in-jerusalem-in-israel-with-behind-204436981.jpg</t>
+  </si>
+  <si>
+    <t>Imagen de Nehru y Ghandi</t>
+  </si>
+  <si>
+    <t>http://thumb101.shutterstock.com/display_pic_with_logo/853195/207003697/stock-photo-india-circa-a-stamp-printed-in-india-shows-gandhi-and-nehru-circa-207003697.jpg</t>
   </si>
 </sst>
 </file>
@@ -830,7 +923,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1010,6 +1103,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1065,7 +1163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1511,17 +1609,63 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1580,7 +1724,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1779,9 +1923,6 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1790,14 +1931,8 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="51"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1884,8 +2019,124 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="51" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="51" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="51" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -2732,11 +2983,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:P108"/>
+  <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.5"/>
@@ -2774,14 +3025,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="F2" s="86" t="s">
+      <c r="D2" s="89"/>
+      <c r="F2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="87"/>
+      <c r="G2" s="82"/>
       <c r="H2" s="50"/>
       <c r="I2" s="50"/>
       <c r="J2" s="15"/>
@@ -2791,14 +3042,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="95">
+      <c r="C3" s="90">
         <v>10</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="F3" s="88">
-        <v>42069</v>
-      </c>
-      <c r="G3" s="89"/>
+      <c r="D3" s="91"/>
+      <c r="F3" s="83">
+        <v>42122</v>
+      </c>
+      <c r="G3" s="84"/>
       <c r="H3" s="50"/>
       <c r="I3" s="50"/>
       <c r="J3" s="15"/>
@@ -2808,10 +3059,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="92" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="96"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="5"/>
       <c r="F4" s="49" t="s">
         <v>55</v>
@@ -2827,10 +3078,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="93" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="99"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="5"/>
       <c r="F5" s="47" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2879,12 +3130,12 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="92"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
       <c r="J8" s="17"/>
       <c r="K8" s="11"/>
       <c r="L8" s="2"/>
@@ -2897,10 +3148,10 @@
       <c r="A9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="127" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="23" t="s">
@@ -2932,19 +3183,19 @@
       <c r="A10" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="117" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="78" t="s">
+      <c r="D10" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F10" s="79" t="s">
+      <c r="F10" s="78" t="s">
         <v>168</v>
       </c>
       <c r="G10" s="13" t="str">
@@ -2959,7 +3210,7 @@
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J10" s="80" t="s">
+      <c r="J10" s="79" t="s">
         <v>169</v>
       </c>
       <c r="K10" s="18"/>
@@ -2968,19 +3219,19 @@
       <c r="A11" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="119" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="78" t="s">
+      <c r="E11" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="78" t="s">
         <v>172</v>
       </c>
       <c r="G11" s="13" t="str">
@@ -2988,14 +3239,14 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H11" s="13" t="str">
-        <f t="shared" ref="H11:H74" si="0">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H11:H85" si="0">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CS_10_01_CO_F02a.png</v>
       </c>
       <c r="I11" s="13" t="str">
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="80" t="s">
+      <c r="J11" s="79" t="s">
         <v>169</v>
       </c>
       <c r="K11" s="14"/>
@@ -3004,22 +3255,22 @@
       <c r="A12" s="75" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="128" t="s">
         <v>176</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="78" t="s">
+      <c r="D12" s="122" t="s">
         <v>166</v>
       </c>
-      <c r="E12" s="78" t="s">
+      <c r="E12" s="122" t="s">
         <v>167</v>
       </c>
-      <c r="F12" s="79" t="s">
+      <c r="F12" s="78" t="s">
         <v>175</v>
       </c>
-      <c r="G12" s="13" t="str">
+      <c r="G12" s="123" t="str">
         <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
@@ -3031,35 +3282,35 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="80" t="s">
+      <c r="J12" s="79" t="s">
         <v>177</v>
       </c>
       <c r="K12" s="18"/>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="243">
-      <c r="A13" s="75" t="s">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="135.75">
+      <c r="A13" s="113" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="118" t="s">
-        <v>241</v>
-      </c>
-      <c r="C13" s="77" t="s">
+      <c r="B13" s="129" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="78" t="s">
+      <c r="D13" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="78" t="s">
+      <c r="E13" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="124" t="s">
         <v>178</v>
       </c>
       <c r="G13" s="13" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H13" s="13" t="str">
+      <c r="H13" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F04a.png</v>
       </c>
@@ -3067,359 +3318,267 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="80" t="s">
+      <c r="J13" s="79" t="s">
+        <v>251</v>
+      </c>
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="135" customHeight="1">
+      <c r="A14" s="143" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="144" t="s">
+        <v>250</v>
+      </c>
+      <c r="C14" s="121" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="122" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="122" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="145"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="146"/>
+      <c r="I14" s="123"/>
+      <c r="J14" s="79" t="s">
+        <v>252</v>
+      </c>
+      <c r="K14" s="147"/>
+    </row>
+    <row r="15" spans="1:16" s="131" customFormat="1" ht="15.75">
+      <c r="A15" s="131" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="134" t="s">
+        <v>253</v>
+      </c>
+      <c r="C15" s="130" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="130" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="130" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" s="156" t="s">
+        <v>254</v>
+      </c>
+      <c r="K15" s="157"/>
+    </row>
+    <row r="16" spans="1:16" s="157" customFormat="1" ht="15.75">
+      <c r="A16" s="158" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="159" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="137"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="156" t="s">
+        <v>256</v>
+      </c>
+      <c r="K16" s="141"/>
+    </row>
+    <row r="17" spans="1:11" s="157" customFormat="1" ht="15.75">
+      <c r="A17" s="158" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="159" t="s">
+        <v>257</v>
+      </c>
+      <c r="C17" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" s="137"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="138"/>
+      <c r="J17" s="160" t="s">
+        <v>258</v>
+      </c>
+      <c r="K17" s="141"/>
+    </row>
+    <row r="18" spans="1:11" s="157" customFormat="1" ht="15.75">
+      <c r="A18" s="158" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="159" t="s">
+        <v>259</v>
+      </c>
+      <c r="C18" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E18" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" s="137"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="138"/>
+      <c r="J18" s="160" t="s">
+        <v>260</v>
+      </c>
+      <c r="K18" s="141"/>
+    </row>
+    <row r="19" spans="1:11" s="157" customFormat="1" ht="15.75">
+      <c r="A19" s="158" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="159" t="s">
+        <v>261</v>
+      </c>
+      <c r="C19" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E19" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F19" s="137"/>
+      <c r="G19" s="138"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="160" t="s">
+        <v>262</v>
+      </c>
+      <c r="K19" s="141"/>
+    </row>
+    <row r="20" spans="1:11" s="157" customFormat="1" ht="15.75">
+      <c r="A20" s="158" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="159" t="s">
+        <v>263</v>
+      </c>
+      <c r="C20" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" s="137"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="160" t="s">
+        <v>264</v>
+      </c>
+      <c r="K20" s="141"/>
+    </row>
+    <row r="21" spans="1:11" s="157" customFormat="1" ht="15.75">
+      <c r="A21" s="158" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="159" t="s">
+        <v>265</v>
+      </c>
+      <c r="C21" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="137"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="138"/>
+      <c r="J21" s="160" t="s">
+        <v>266</v>
+      </c>
+      <c r="K21" s="141"/>
+    </row>
+    <row r="22" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A22" s="148" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="149" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="150" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="151" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="151" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" s="152" t="s">
         <v>179</v>
       </c>
-      <c r="K13" s="18"/>
-    </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="15.75">
-      <c r="A14" s="75" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" s="76" t="s">
-        <v>173</v>
-      </c>
-      <c r="C14" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F14" s="79" t="s">
-        <v>180</v>
-      </c>
-      <c r="G14" s="13" t="str">
-        <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H14" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F05a.png</v>
-      </c>
-      <c r="I14" s="13" t="str">
-        <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J14" s="80" t="s">
-        <v>181</v>
-      </c>
-      <c r="K14" s="18"/>
-    </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="15.75">
-      <c r="A15" s="75" t="s">
-        <v>153</v>
-      </c>
-      <c r="B15" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E15" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F15" s="79" t="s">
-        <v>183</v>
-      </c>
-      <c r="G15" s="13" t="str">
-        <f>IF(F15&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H15" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F06a.png</v>
-      </c>
-      <c r="I15" s="13" t="str">
-        <f>IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J15" s="80" t="s">
-        <v>184</v>
-      </c>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="16.5">
-      <c r="A16" s="75" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="81" t="s">
-        <v>185</v>
-      </c>
-      <c r="C16" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E16" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" s="79" t="s">
-        <v>186</v>
-      </c>
-      <c r="G16" s="13" t="str">
-        <f>IF(F16&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H16" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F07a.png</v>
-      </c>
-      <c r="I16" s="13" t="str">
-        <f>IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J16" s="80" t="s">
-        <v>187</v>
-      </c>
-      <c r="K16" s="31"/>
-    </row>
-    <row r="17" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A17" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="81" t="s">
-        <v>188</v>
-      </c>
-      <c r="C17" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F17" s="79" t="s">
-        <v>189</v>
-      </c>
-      <c r="G17" s="13" t="str">
-        <f>IF(F17&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H17" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F08a.png</v>
-      </c>
-      <c r="I17" s="13" t="str">
-        <f>IF(OR(B17&lt;&gt;"",J17&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J17" s="80" t="s">
-        <v>190</v>
-      </c>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A18" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" s="81" t="s">
-        <v>191</v>
-      </c>
-      <c r="C18" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E18" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F18" s="79" t="s">
-        <v>192</v>
-      </c>
-      <c r="G18" s="13" t="str">
-        <f>IF(F18&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H18" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F09a.png</v>
-      </c>
-      <c r="I18" s="13" t="str">
-        <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J18" s="80" t="s">
-        <v>193</v>
-      </c>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="1:11" s="11" customFormat="1" ht="16.5">
-      <c r="A19" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="B19" s="81" t="s">
-        <v>194</v>
-      </c>
-      <c r="C19" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E19" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F19" s="79" t="s">
-        <v>195</v>
-      </c>
-      <c r="G19" s="13" t="str">
-        <f>IF(F19&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H19" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F10a.png</v>
-      </c>
-      <c r="I19" s="13" t="str">
-        <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J19" s="80" t="s">
-        <v>196</v>
-      </c>
-      <c r="K19" s="31"/>
-    </row>
-    <row r="20" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A20" s="75" t="s">
-        <v>158</v>
-      </c>
-      <c r="B20" s="81" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F20" s="79" t="s">
-        <v>198</v>
-      </c>
-      <c r="G20" s="13" t="str">
-        <f>IF(F20&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H20" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F11a.png</v>
-      </c>
-      <c r="I20" s="13" t="str">
-        <f>IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J20" s="80" t="s">
-        <v>199</v>
-      </c>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A21" s="75" t="s">
-        <v>159</v>
-      </c>
-      <c r="B21" s="83" t="s">
-        <v>200</v>
-      </c>
-      <c r="C21" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F21" s="79" t="s">
-        <v>201</v>
-      </c>
-      <c r="G21" s="13" t="str">
-        <f>IF(F21&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H21" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F12a.png</v>
-      </c>
-      <c r="I21" s="13" t="str">
-        <f>IF(OR(B21&lt;&gt;"",J21&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J21" s="80" t="s">
-        <v>202</v>
-      </c>
-      <c r="K21" s="20"/>
-    </row>
-    <row r="22" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A22" s="75" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="81" t="s">
-        <v>203</v>
-      </c>
-      <c r="C22" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E22" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="79" t="s">
-        <v>204</v>
-      </c>
-      <c r="G22" s="13" t="str">
+      <c r="G22" s="153" t="str">
         <f>IF(F22&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H22" s="13" t="str">
-        <f t="shared" si="0"/>
+      <c r="H22" s="154" t="str">
+        <f>IF(AND(I22&lt;&gt;"",I22&lt;&gt;0),IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),CONCATENATE($C$7,"_",$A22,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CS_10_01_CO_F13a.png</v>
       </c>
-      <c r="I22" s="13" t="str">
+      <c r="I22" s="153" t="str">
         <f>IF(OR(B22&lt;&gt;"",J22&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J22" s="80" t="s">
-        <v>205</v>
-      </c>
-      <c r="K22" s="19"/>
+      <c r="J22" s="79" t="s">
+        <v>180</v>
+      </c>
+      <c r="K22" s="155"/>
     </row>
     <row r="23" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="113" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="81" t="s">
-        <v>206</v>
-      </c>
-      <c r="C23" s="77" t="s">
+      <c r="B23" s="118" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="78" t="s">
+      <c r="D23" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="78" t="s">
+      <c r="E23" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F23" s="79" t="s">
-        <v>207</v>
+      <c r="F23" s="124" t="s">
+        <v>182</v>
       </c>
       <c r="G23" s="13" t="str">
         <f>IF(F23&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H23" s="13" t="str">
+      <c r="H23" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F14a.png</v>
       </c>
@@ -3427,71 +3586,60 @@
         <f>IF(OR(B23&lt;&gt;"",J23&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J23" s="80" t="s">
-        <v>208</v>
-      </c>
-      <c r="K23" s="18"/>
-    </row>
-    <row r="24" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A24" s="75" t="s">
+      <c r="J23" s="79" t="s">
+        <v>183</v>
+      </c>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" s="132" customFormat="1" ht="15.75">
+      <c r="A24" s="133" t="s">
         <v>161</v>
       </c>
-      <c r="B24" s="81" t="s">
-        <v>209</v>
-      </c>
-      <c r="C24" s="77" t="s">
+      <c r="B24" s="142" t="s">
+        <v>267</v>
+      </c>
+      <c r="C24" s="135" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="78" t="s">
+      <c r="D24" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="E24" s="78" t="s">
+      <c r="E24" s="136" t="s">
         <v>167</v>
       </c>
-      <c r="F24" s="79" t="s">
-        <v>210</v>
-      </c>
-      <c r="G24" s="13" t="str">
-        <f>IF(F24&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H24" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F15a.png</v>
-      </c>
-      <c r="I24" s="13" t="str">
-        <f>IF(OR(B24&lt;&gt;"",J24&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J24" s="80" t="s">
-        <v>211</v>
-      </c>
-      <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A25" s="75" t="s">
+      <c r="F24" s="137"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="139"/>
+      <c r="I24" s="138"/>
+      <c r="J24" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="K24" s="161"/>
+    </row>
+    <row r="25" spans="1:11" s="11" customFormat="1" ht="16.5">
+      <c r="A25" s="113" t="s">
         <v>162</v>
       </c>
-      <c r="B25" s="81" t="s">
-        <v>212</v>
-      </c>
-      <c r="C25" s="77" t="s">
+      <c r="B25" s="118" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="78" t="s">
+      <c r="D25" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E25" s="78" t="s">
+      <c r="E25" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F25" s="79" t="s">
-        <v>213</v>
+      <c r="F25" s="124" t="s">
+        <v>185</v>
       </c>
       <c r="G25" s="13" t="str">
         <f>IF(F25&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H25" s="13" t="str">
+      <c r="H25" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F16a.png</v>
       </c>
@@ -3499,35 +3647,35 @@
         <f>IF(OR(B25&lt;&gt;"",J25&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J25" s="80" t="s">
-        <v>214</v>
-      </c>
-      <c r="K25" s="18"/>
+      <c r="J25" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="K25" s="31"/>
     </row>
     <row r="26" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="113" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="81" t="s">
-        <v>215</v>
-      </c>
-      <c r="C26" s="77" t="s">
+      <c r="B26" s="118" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="78" t="s">
+      <c r="D26" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E26" s="78" t="s">
+      <c r="E26" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F26" s="79" t="s">
-        <v>216</v>
+      <c r="F26" s="124" t="s">
+        <v>188</v>
       </c>
       <c r="G26" s="13" t="str">
         <f>IF(F26&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H26" s="13" t="str">
+      <c r="H26" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F17a.png</v>
       </c>
@@ -3535,35 +3683,35 @@
         <f>IF(OR(B26&lt;&gt;"",J26&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J26" s="80" t="s">
-        <v>217</v>
-      </c>
-      <c r="K26" s="18"/>
+      <c r="J26" s="79" t="s">
+        <v>189</v>
+      </c>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="113" t="s">
         <v>164</v>
       </c>
-      <c r="B27" s="81" t="s">
-        <v>218</v>
-      </c>
-      <c r="C27" s="77" t="s">
+      <c r="B27" s="118" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="78" t="s">
+      <c r="D27" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E27" s="78" t="s">
+      <c r="E27" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F27" s="79" t="s">
-        <v>219</v>
+      <c r="F27" s="124" t="s">
+        <v>191</v>
       </c>
       <c r="G27" s="13" t="str">
         <f>IF(F27&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H27" s="13" t="str">
+      <c r="H27" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F18a.png</v>
       </c>
@@ -3571,35 +3719,35 @@
         <f>IF(OR(B27&lt;&gt;"",J27&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J27" s="80" t="s">
-        <v>220</v>
-      </c>
-      <c r="K27" s="18"/>
-    </row>
-    <row r="28" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A28" s="75" t="s">
+      <c r="J27" s="79" t="s">
+        <v>192</v>
+      </c>
+      <c r="K27" s="20"/>
+    </row>
+    <row r="28" spans="1:11" s="11" customFormat="1" ht="16.5">
+      <c r="A28" s="113" t="s">
         <v>165</v>
       </c>
-      <c r="B28" s="81" t="s">
-        <v>221</v>
-      </c>
-      <c r="C28" s="77" t="s">
+      <c r="B28" s="118" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="78" t="s">
+      <c r="D28" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E28" s="78" t="s">
+      <c r="E28" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F28" s="79" t="s">
-        <v>228</v>
+      <c r="F28" s="124" t="s">
+        <v>194</v>
       </c>
       <c r="G28" s="13" t="str">
         <f>IF(F28&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H28" s="13" t="str">
+      <c r="H28" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F19a.png</v>
       </c>
@@ -3607,35 +3755,35 @@
         <f>IF(OR(B28&lt;&gt;"",J28&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J28" s="80" t="s">
-        <v>229</v>
-      </c>
-      <c r="K28" s="18"/>
+      <c r="J28" s="79" t="s">
+        <v>195</v>
+      </c>
+      <c r="K28" s="31"/>
     </row>
     <row r="29" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A29" s="75" t="s">
-        <v>222</v>
-      </c>
-      <c r="B29" s="81" t="s">
-        <v>230</v>
-      </c>
-      <c r="C29" s="77" t="s">
+      <c r="A29" s="113" t="s">
+        <v>221</v>
+      </c>
+      <c r="B29" s="118" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="78" t="s">
+      <c r="D29" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E29" s="78" t="s">
+      <c r="E29" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F29" s="79" t="s">
-        <v>231</v>
+      <c r="F29" s="124" t="s">
+        <v>197</v>
       </c>
       <c r="G29" s="13" t="str">
         <f>IF(F29&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H29" s="13" t="str">
+      <c r="H29" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F20a.png</v>
       </c>
@@ -3643,71 +3791,60 @@
         <f>IF(OR(B29&lt;&gt;"",J29&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J29" s="80" t="s">
-        <v>232</v>
-      </c>
-      <c r="K29" s="18"/>
-    </row>
-    <row r="30" spans="1:11" s="11" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A30" s="75" t="s">
+      <c r="J29" s="79" t="s">
+        <v>198</v>
+      </c>
+      <c r="K29" s="20"/>
+    </row>
+    <row r="30" spans="1:11" s="132" customFormat="1" ht="15.75">
+      <c r="A30" s="133" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="142" t="s">
+        <v>270</v>
+      </c>
+      <c r="C30" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E30" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F30" s="137"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="139"/>
+      <c r="I30" s="138"/>
+      <c r="J30" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="K30" s="161"/>
+    </row>
+    <row r="31" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A31" s="113" t="s">
         <v>223</v>
       </c>
-      <c r="B30" s="81" t="s">
-        <v>233</v>
-      </c>
-      <c r="C30" s="77" t="s">
+      <c r="B31" s="119" t="s">
+        <v>199</v>
+      </c>
+      <c r="C31" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="78" t="s">
+      <c r="D31" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="78" t="s">
+      <c r="E31" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F30" s="79" t="s">
-        <v>234</v>
-      </c>
-      <c r="G30" s="13" t="str">
-        <f>IF(F30&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
-      </c>
-      <c r="H30" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>CS_10_01_CO_F21a.png</v>
-      </c>
-      <c r="I30" s="13" t="str">
-        <f>IF(OR(B30&lt;&gt;"",J30&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J30" s="80" t="s">
-        <v>235</v>
-      </c>
-      <c r="K30" s="18"/>
-    </row>
-    <row r="31" spans="1:11" s="11" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A31" s="75" t="s">
-        <v>224</v>
-      </c>
-      <c r="B31" s="84" t="s">
-        <v>236</v>
-      </c>
-      <c r="C31" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="D31" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E31" s="78" t="s">
-        <v>167</v>
-      </c>
-      <c r="F31" s="85" t="s">
-        <v>237</v>
+      <c r="F31" s="124" t="s">
+        <v>200</v>
       </c>
       <c r="G31" s="13" t="str">
         <f>IF(F31&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H31" s="13" t="str">
+      <c r="H31" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F22a.png</v>
       </c>
@@ -3715,35 +3852,35 @@
         <f>IF(OR(B31&lt;&gt;"",J31&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J31" s="80" t="s">
-        <v>238</v>
-      </c>
-      <c r="K31" s="18"/>
+      <c r="J31" s="79" t="s">
+        <v>201</v>
+      </c>
+      <c r="K31" s="20"/>
     </row>
     <row r="32" spans="1:11" s="11" customFormat="1" ht="15.75">
-      <c r="A32" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="B32" s="81" t="s">
-        <v>171</v>
-      </c>
-      <c r="C32" s="77" t="s">
+      <c r="A32" s="113" t="s">
+        <v>224</v>
+      </c>
+      <c r="B32" s="118" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="78" t="s">
+      <c r="D32" s="77" t="s">
         <v>166</v>
       </c>
-      <c r="E32" s="78" t="s">
+      <c r="E32" s="77" t="s">
         <v>167</v>
       </c>
-      <c r="F32" s="79" t="s">
-        <v>239</v>
+      <c r="F32" s="124" t="s">
+        <v>203</v>
       </c>
       <c r="G32" s="13" t="str">
         <f>IF(F32&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H32" s="13" t="str">
+      <c r="H32" s="120" t="str">
         <f t="shared" si="0"/>
         <v>CS_10_01_CO_F23a.png</v>
       </c>
@@ -3751,281 +3888,408 @@
         <f>IF(OR(B32&lt;&gt;"",J32&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J32" s="80" t="s">
+      <c r="J32" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="K32" s="19"/>
+    </row>
+    <row r="33" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A33" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="K32" s="18"/>
-    </row>
-    <row r="33" spans="1:11" s="11" customFormat="1">
-      <c r="A33" s="75"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="13"/>
+      <c r="B33" s="118" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F33" s="124" t="s">
+        <v>206</v>
+      </c>
       <c r="G33" s="13" t="str">
         <f>IF(F33&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H33" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H33" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F24a.png</v>
       </c>
       <c r="I33" s="13" t="str">
         <f>IF(OR(B33&lt;&gt;"",J33&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J33" s="18"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J33" s="79" t="s">
+        <v>207</v>
+      </c>
       <c r="K33" s="18"/>
     </row>
-    <row r="34" spans="1:11" s="11" customFormat="1">
-      <c r="A34" s="75"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="13"/>
+    <row r="34" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A34" s="113" t="s">
+        <v>241</v>
+      </c>
+      <c r="B34" s="118" t="s">
+        <v>208</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F34" s="124" t="s">
+        <v>209</v>
+      </c>
       <c r="G34" s="13" t="str">
         <f>IF(F34&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H34" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H34" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F25a.png</v>
       </c>
       <c r="I34" s="13" t="str">
         <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-    </row>
-    <row r="35" spans="1:11" s="11" customFormat="1">
-      <c r="A35" s="75"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="78"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J34" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="K34" s="14"/>
+    </row>
+    <row r="35" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A35" s="113" t="s">
+        <v>242</v>
+      </c>
+      <c r="B35" s="118" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="124" t="s">
+        <v>212</v>
+      </c>
       <c r="G35" s="13" t="str">
         <f>IF(F35&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H35" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H35" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F26a.png</v>
       </c>
       <c r="I35" s="13" t="str">
         <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J35" s="13"/>
-      <c r="K35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" s="11" customFormat="1">
-      <c r="A36" s="75"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J35" s="79" t="s">
+        <v>213</v>
+      </c>
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A36" s="113" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="118" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F36" s="124" t="s">
+        <v>215</v>
+      </c>
       <c r="G36" s="13" t="str">
         <f>IF(F36&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H36" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H36" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F27a.png</v>
       </c>
       <c r="I36" s="13" t="str">
         <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J36" s="13"/>
-      <c r="K36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" s="11" customFormat="1">
-      <c r="A37" s="75"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J36" s="79" t="s">
+        <v>216</v>
+      </c>
+      <c r="K36" s="18"/>
+    </row>
+    <row r="37" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A37" s="113" t="s">
+        <v>244</v>
+      </c>
+      <c r="B37" s="118" t="s">
+        <v>217</v>
+      </c>
+      <c r="C37" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="124" t="s">
+        <v>218</v>
+      </c>
       <c r="G37" s="13" t="str">
         <f>IF(F37&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H37" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H37" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F28a.png</v>
       </c>
       <c r="I37" s="13" t="str">
         <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J37" s="21"/>
-      <c r="K37" s="14"/>
-    </row>
-    <row r="38" spans="1:11" s="11" customFormat="1">
-      <c r="A38" s="75"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="78"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13" t="str">
-        <f>IF(F38&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H38" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I38" s="13" t="str">
-        <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J38" s="22"/>
-      <c r="K38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" s="11" customFormat="1">
-      <c r="A39" s="75"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="78"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J37" s="79" t="s">
+        <v>219</v>
+      </c>
+      <c r="K37" s="18"/>
+    </row>
+    <row r="38" spans="1:11" s="132" customFormat="1" ht="15.75">
+      <c r="A38" s="133" t="s">
+        <v>245</v>
+      </c>
+      <c r="B38" s="142" t="s">
+        <v>272</v>
+      </c>
+      <c r="C38" s="135" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="136" t="s">
+        <v>166</v>
+      </c>
+      <c r="E38" s="136" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" s="137"/>
+      <c r="G38" s="138"/>
+      <c r="H38" s="139"/>
+      <c r="I38" s="138"/>
+      <c r="J38" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="K38" s="141"/>
+    </row>
+    <row r="39" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A39" s="113" t="s">
+        <v>246</v>
+      </c>
+      <c r="B39" s="118" t="s">
+        <v>220</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E39" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="124" t="s">
+        <v>227</v>
+      </c>
       <c r="G39" s="13" t="str">
         <f>IF(F39&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H39" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H39" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F30a.png</v>
       </c>
       <c r="I39" s="13" t="str">
         <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J39" s="13"/>
-      <c r="K39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" s="11" customFormat="1">
-      <c r="A40" s="75"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="13"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J39" s="79" t="s">
+        <v>228</v>
+      </c>
+      <c r="K39" s="18"/>
+    </row>
+    <row r="40" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A40" s="113" t="s">
+        <v>247</v>
+      </c>
+      <c r="B40" s="118" t="s">
+        <v>229</v>
+      </c>
+      <c r="C40" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" s="124" t="s">
+        <v>230</v>
+      </c>
       <c r="G40" s="13" t="str">
         <f>IF(F40&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H40" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H40" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F31a.png</v>
       </c>
       <c r="I40" s="13" t="str">
         <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J40" s="13"/>
-      <c r="K40" s="14"/>
-    </row>
-    <row r="41" spans="1:11" s="11" customFormat="1">
-      <c r="A41" s="75" t="s">
-        <v>226</v>
-      </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13" t="str">
-        <f t="shared" ref="F41:F74" si="1">IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),CONCATENATE($C$7,"_",$A41,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I41="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J40" s="79" t="s">
+        <v>231</v>
+      </c>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A41" s="113" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="118" t="s">
+        <v>232</v>
+      </c>
+      <c r="C41" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E41" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" s="124" t="s">
+        <v>233</v>
       </c>
       <c r="G41" s="13" t="str">
         <f>IF(F41&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H41" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H41" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F32a.png</v>
       </c>
       <c r="I41" s="13" t="str">
         <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J41" s="13"/>
-      <c r="K41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" s="11" customFormat="1">
-      <c r="A42" s="75" t="s">
-        <v>227</v>
-      </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J41" s="79" t="s">
+        <v>234</v>
+      </c>
+      <c r="K41" s="18"/>
+    </row>
+    <row r="42" spans="1:11" s="11" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A42" s="113" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="80" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" s="125" t="s">
+        <v>236</v>
       </c>
       <c r="G42" s="13" t="str">
         <f>IF(F42&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H42" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H42" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F33a.png</v>
       </c>
       <c r="I42" s="13" t="str">
         <f>IF(OR(B42&lt;&gt;"",J42&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J42" s="13"/>
-      <c r="K42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" s="11" customFormat="1">
-      <c r="A43" s="12"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J42" s="79" t="s">
+        <v>237</v>
+      </c>
+      <c r="K42" s="18"/>
+    </row>
+    <row r="43" spans="1:11" s="11" customFormat="1" ht="15.75">
+      <c r="A43" s="113" t="s">
+        <v>248</v>
+      </c>
+      <c r="B43" s="118" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E43" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="F43" s="124" t="s">
+        <v>238</v>
       </c>
       <c r="G43" s="13" t="str">
         <f>IF(F43&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H43" s="13" t="str">
+        <v>526 x 370 px</v>
+      </c>
+      <c r="H43" s="120" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>CS_10_01_CO_F34a.png</v>
       </c>
       <c r="I43" s="13" t="str">
         <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J43" s="13"/>
-      <c r="K43" s="14"/>
+        <v>800 x 600 px</v>
+      </c>
+      <c r="J43" s="79" t="s">
+        <v>239</v>
+      </c>
+      <c r="K43" s="18"/>
     </row>
     <row r="44" spans="1:11" s="11" customFormat="1">
-      <c r="A44" s="12"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A44" s="113"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="13" t="str">
         <f>IF(F44&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H44" s="13" t="str">
+      <c r="H44" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4033,24 +4297,21 @@
         <f>IF(OR(B44&lt;&gt;"",J44&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J44" s="13"/>
-      <c r="K44" s="14"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
     </row>
     <row r="45" spans="1:11" s="11" customFormat="1">
-      <c r="A45" s="12"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A45" s="113"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="77"/>
+      <c r="E45" s="77"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="13" t="str">
         <f>IF(F45&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H45" s="13" t="str">
+      <c r="H45" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4058,24 +4319,21 @@
         <f>IF(OR(B45&lt;&gt;"",J45&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J45" s="13"/>
-      <c r="K45" s="14"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
     </row>
     <row r="46" spans="1:11" s="11" customFormat="1">
-      <c r="A46" s="12"/>
+      <c r="A46" s="113"/>
       <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="C46" s="76"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
+      <c r="F46" s="13"/>
       <c r="G46" s="13" t="str">
         <f>IF(F46&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H46" s="13" t="str">
+      <c r="H46" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4087,20 +4345,17 @@
       <c r="K46" s="14"/>
     </row>
     <row r="47" spans="1:11" s="11" customFormat="1">
-      <c r="A47" s="12"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A47" s="113"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="77"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="13"/>
       <c r="G47" s="13" t="str">
         <f>IF(F47&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H47" s="13" t="str">
+      <c r="H47" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4112,20 +4367,17 @@
       <c r="K47" s="14"/>
     </row>
     <row r="48" spans="1:11" s="11" customFormat="1">
-      <c r="A48" s="12"/>
+      <c r="A48" s="113"/>
       <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="C48" s="76"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="13" t="str">
         <f>IF(F48&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H48" s="13" t="str">
+      <c r="H48" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4133,24 +4385,21 @@
         <f>IF(OR(B48&lt;&gt;"",J48&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J48" s="13"/>
+      <c r="J48" s="21"/>
       <c r="K48" s="14"/>
     </row>
     <row r="49" spans="1:11" s="11" customFormat="1">
-      <c r="A49" s="12"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A49" s="113"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="13"/>
       <c r="G49" s="13" t="str">
         <f>IF(F49&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H49" s="13" t="str">
+      <c r="H49" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4158,24 +4407,21 @@
         <f>IF(OR(B49&lt;&gt;"",J49&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
-      <c r="J49" s="13"/>
+      <c r="J49" s="22"/>
       <c r="K49" s="14"/>
     </row>
     <row r="50" spans="1:11" s="11" customFormat="1">
-      <c r="A50" s="12"/>
+      <c r="A50" s="113"/>
       <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="C50" s="76"/>
+      <c r="D50" s="77"/>
+      <c r="E50" s="77"/>
+      <c r="F50" s="13"/>
       <c r="G50" s="13" t="str">
         <f>IF(F50&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H50" s="13" t="str">
+      <c r="H50" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4187,20 +4433,17 @@
       <c r="K50" s="14"/>
     </row>
     <row r="51" spans="1:11" s="11" customFormat="1">
-      <c r="A51" s="12"/>
+      <c r="A51" s="113"/>
       <c r="B51" s="26"/>
       <c r="C51" s="26"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="E51" s="77"/>
+      <c r="F51" s="13"/>
       <c r="G51" s="13" t="str">
         <f>IF(F51&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H51" s="13" t="str">
+      <c r="H51" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4212,20 +4455,20 @@
       <c r="K51" s="14"/>
     </row>
     <row r="52" spans="1:11" s="11" customFormat="1">
-      <c r="A52" s="12"/>
+      <c r="A52" s="113"/>
       <c r="B52" s="26"/>
       <c r="C52" s="26"/>
       <c r="D52" s="13"/>
       <c r="E52" s="13"/>
       <c r="F52" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F52:F85" si="1">IF(OR(B52&lt;&gt;"",J52&lt;&gt;""),CONCATENATE($C$7,"_",$A52,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I52="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G52" s="13" t="str">
         <f>IF(F52&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H52" s="13" t="str">
+      <c r="H52" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4237,7 +4480,7 @@
       <c r="K52" s="14"/>
     </row>
     <row r="53" spans="1:11" s="11" customFormat="1">
-      <c r="A53" s="12"/>
+      <c r="A53" s="113"/>
       <c r="B53" s="26"/>
       <c r="C53" s="26"/>
       <c r="D53" s="13"/>
@@ -4250,7 +4493,7 @@
         <f>IF(F53&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H53" s="13" t="str">
+      <c r="H53" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4262,7 +4505,7 @@
       <c r="K53" s="14"/>
     </row>
     <row r="54" spans="1:11" s="11" customFormat="1">
-      <c r="A54" s="12"/>
+      <c r="A54" s="114"/>
       <c r="B54" s="26"/>
       <c r="C54" s="26"/>
       <c r="D54" s="13"/>
@@ -4275,7 +4518,7 @@
         <f>IF(F54&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H54" s="13" t="str">
+      <c r="H54" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4287,7 +4530,7 @@
       <c r="K54" s="14"/>
     </row>
     <row r="55" spans="1:11" s="11" customFormat="1">
-      <c r="A55" s="12"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="26"/>
       <c r="C55" s="26"/>
       <c r="D55" s="13"/>
@@ -4300,7 +4543,7 @@
         <f>IF(F55&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H55" s="13" t="str">
+      <c r="H55" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4312,7 +4555,7 @@
       <c r="K55" s="14"/>
     </row>
     <row r="56" spans="1:11" s="11" customFormat="1">
-      <c r="A56" s="12"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="26"/>
       <c r="C56" s="26"/>
       <c r="D56" s="13"/>
@@ -4325,7 +4568,7 @@
         <f>IF(F56&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H56" s="13" t="str">
+      <c r="H56" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4337,7 +4580,7 @@
       <c r="K56" s="14"/>
     </row>
     <row r="57" spans="1:11" s="11" customFormat="1">
-      <c r="A57" s="12"/>
+      <c r="A57" s="114"/>
       <c r="B57" s="26"/>
       <c r="C57" s="26"/>
       <c r="D57" s="13"/>
@@ -4350,7 +4593,7 @@
         <f>IF(F57&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H57" s="13" t="str">
+      <c r="H57" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4362,7 +4605,7 @@
       <c r="K57" s="14"/>
     </row>
     <row r="58" spans="1:11" s="11" customFormat="1">
-      <c r="A58" s="12"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="26"/>
       <c r="C58" s="26"/>
       <c r="D58" s="13"/>
@@ -4375,7 +4618,7 @@
         <f>IF(F58&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H58" s="13" t="str">
+      <c r="H58" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4387,7 +4630,7 @@
       <c r="K58" s="14"/>
     </row>
     <row r="59" spans="1:11" s="11" customFormat="1">
-      <c r="A59" s="12"/>
+      <c r="A59" s="114"/>
       <c r="B59" s="26"/>
       <c r="C59" s="26"/>
       <c r="D59" s="13"/>
@@ -4400,7 +4643,7 @@
         <f>IF(F59&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H59" s="13" t="str">
+      <c r="H59" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4412,7 +4655,7 @@
       <c r="K59" s="14"/>
     </row>
     <row r="60" spans="1:11" s="11" customFormat="1">
-      <c r="A60" s="12"/>
+      <c r="A60" s="114"/>
       <c r="B60" s="26"/>
       <c r="C60" s="26"/>
       <c r="D60" s="13"/>
@@ -4425,7 +4668,7 @@
         <f>IF(F60&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H60" s="13" t="str">
+      <c r="H60" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4437,7 +4680,7 @@
       <c r="K60" s="14"/>
     </row>
     <row r="61" spans="1:11" s="11" customFormat="1">
-      <c r="A61" s="12"/>
+      <c r="A61" s="114"/>
       <c r="B61" s="26"/>
       <c r="C61" s="26"/>
       <c r="D61" s="13"/>
@@ -4450,7 +4693,7 @@
         <f>IF(F61&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H61" s="13" t="str">
+      <c r="H61" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4462,9 +4705,9 @@
       <c r="K61" s="14"/>
     </row>
     <row r="62" spans="1:11" s="11" customFormat="1">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
+      <c r="A62" s="114"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
       <c r="F62" s="13" t="str">
@@ -4475,7 +4718,7 @@
         <f>IF(F62&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H62" s="13" t="str">
+      <c r="H62" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4487,9 +4730,9 @@
       <c r="K62" s="14"/>
     </row>
     <row r="63" spans="1:11" s="11" customFormat="1">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
+      <c r="A63" s="114"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
       <c r="F63" s="13" t="str">
@@ -4500,7 +4743,7 @@
         <f>IF(F63&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H63" s="13" t="str">
+      <c r="H63" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4512,9 +4755,9 @@
       <c r="K63" s="14"/>
     </row>
     <row r="64" spans="1:11" s="11" customFormat="1">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
+      <c r="A64" s="114"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
       <c r="D64" s="13"/>
       <c r="E64" s="13"/>
       <c r="F64" s="13" t="str">
@@ -4525,7 +4768,7 @@
         <f>IF(F64&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H64" s="13" t="str">
+      <c r="H64" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4537,9 +4780,9 @@
       <c r="K64" s="14"/>
     </row>
     <row r="65" spans="1:11" s="11" customFormat="1">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
+      <c r="A65" s="114"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
       <c r="D65" s="13"/>
       <c r="E65" s="13"/>
       <c r="F65" s="13" t="str">
@@ -4550,7 +4793,7 @@
         <f>IF(F65&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H65" s="13" t="str">
+      <c r="H65" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4562,9 +4805,9 @@
       <c r="K65" s="14"/>
     </row>
     <row r="66" spans="1:11" s="11" customFormat="1">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
+      <c r="A66" s="114"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
       <c r="F66" s="13" t="str">
@@ -4575,7 +4818,7 @@
         <f>IF(F66&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
         <v/>
       </c>
-      <c r="H66" s="13" t="str">
+      <c r="H66" s="120" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4587,9 +4830,9 @@
       <c r="K66" s="14"/>
     </row>
     <row r="67" spans="1:11" s="11" customFormat="1">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12"/>
+      <c r="A67" s="114"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="115"/>
       <c r="D67" s="13"/>
       <c r="E67" s="13"/>
       <c r="F67" s="13" t="str">
@@ -4612,9 +4855,9 @@
       <c r="K67" s="14"/>
     </row>
     <row r="68" spans="1:11" s="11" customFormat="1">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
+      <c r="A68" s="114"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="115"/>
       <c r="D68" s="13"/>
       <c r="E68" s="13"/>
       <c r="F68" s="13" t="str">
@@ -4637,9 +4880,9 @@
       <c r="K68" s="14"/>
     </row>
     <row r="69" spans="1:11" s="11" customFormat="1">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
+      <c r="A69" s="114"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="115"/>
       <c r="D69" s="13"/>
       <c r="E69" s="13"/>
       <c r="F69" s="13" t="str">
@@ -4662,9 +4905,9 @@
       <c r="K69" s="14"/>
     </row>
     <row r="70" spans="1:11" s="11" customFormat="1">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
+      <c r="A70" s="114"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="115"/>
       <c r="D70" s="13"/>
       <c r="E70" s="13"/>
       <c r="F70" s="13" t="str">
@@ -4687,9 +4930,9 @@
       <c r="K70" s="14"/>
     </row>
     <row r="71" spans="1:11" s="11" customFormat="1">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
+      <c r="A71" s="114"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="115"/>
       <c r="D71" s="13"/>
       <c r="E71" s="13"/>
       <c r="F71" s="13" t="str">
@@ -4712,9 +4955,9 @@
       <c r="K71" s="14"/>
     </row>
     <row r="72" spans="1:11" s="11" customFormat="1">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
+      <c r="A72" s="114"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="115"/>
       <c r="D72" s="13"/>
       <c r="E72" s="13"/>
       <c r="F72" s="13" t="str">
@@ -4737,9 +4980,9 @@
       <c r="K72" s="14"/>
     </row>
     <row r="73" spans="1:11" s="11" customFormat="1">
-      <c r="A73" s="12"/>
+      <c r="A73" s="114"/>
       <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
+      <c r="C73" s="116"/>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="13" t="str">
@@ -4762,9 +5005,9 @@
       <c r="K73" s="14"/>
     </row>
     <row r="74" spans="1:11" s="11" customFormat="1">
-      <c r="A74" s="12"/>
+      <c r="A74" s="114"/>
       <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
+      <c r="C74" s="116"/>
       <c r="D74" s="13"/>
       <c r="E74" s="13"/>
       <c r="F74" s="13" t="str">
@@ -4787,13 +5030,13 @@
       <c r="K74" s="14"/>
     </row>
     <row r="75" spans="1:11" s="11" customFormat="1">
-      <c r="A75" s="12"/>
+      <c r="A75" s="114"/>
       <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
+      <c r="C75" s="116"/>
       <c r="D75" s="13"/>
       <c r="E75" s="13"/>
       <c r="F75" s="13" t="str">
-        <f t="shared" ref="F75:F108" si="2">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I75="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G75" s="13" t="str">
@@ -4801,7 +5044,7 @@
         <v/>
       </c>
       <c r="H75" s="13" t="str">
-        <f t="shared" ref="H75:H108" si="3">IF(AND(I75&lt;&gt;"",I75&lt;&gt;0),IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),CONCATENATE($C$7,"_",$A75,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I75" s="13" t="str">
@@ -4812,13 +5055,13 @@
       <c r="K75" s="14"/>
     </row>
     <row r="76" spans="1:11" s="11" customFormat="1">
-      <c r="A76" s="12"/>
+      <c r="A76" s="114"/>
       <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
+      <c r="C76" s="116"/>
       <c r="D76" s="13"/>
       <c r="E76" s="13"/>
       <c r="F76" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G76" s="13" t="str">
@@ -4826,7 +5069,7 @@
         <v/>
       </c>
       <c r="H76" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I76" s="13" t="str">
@@ -4837,13 +5080,13 @@
       <c r="K76" s="14"/>
     </row>
     <row r="77" spans="1:11" s="11" customFormat="1">
-      <c r="A77" s="12"/>
+      <c r="A77" s="114"/>
       <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
+      <c r="C77" s="116"/>
       <c r="D77" s="13"/>
       <c r="E77" s="13"/>
       <c r="F77" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G77" s="13" t="str">
@@ -4851,7 +5094,7 @@
         <v/>
       </c>
       <c r="H77" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I77" s="13" t="str">
@@ -4862,13 +5105,13 @@
       <c r="K77" s="14"/>
     </row>
     <row r="78" spans="1:11" s="11" customFormat="1">
-      <c r="A78" s="12"/>
+      <c r="A78" s="114"/>
       <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
+      <c r="C78" s="116"/>
       <c r="D78" s="13"/>
       <c r="E78" s="13"/>
       <c r="F78" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G78" s="13" t="str">
@@ -4876,7 +5119,7 @@
         <v/>
       </c>
       <c r="H78" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I78" s="13" t="str">
@@ -4887,13 +5130,13 @@
       <c r="K78" s="14"/>
     </row>
     <row r="79" spans="1:11" s="11" customFormat="1">
-      <c r="A79" s="12"/>
+      <c r="A79" s="114"/>
       <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
+      <c r="C79" s="116"/>
       <c r="D79" s="13"/>
       <c r="E79" s="13"/>
       <c r="F79" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G79" s="13" t="str">
@@ -4901,7 +5144,7 @@
         <v/>
       </c>
       <c r="H79" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I79" s="13" t="str">
@@ -4912,13 +5155,13 @@
       <c r="K79" s="14"/>
     </row>
     <row r="80" spans="1:11" s="11" customFormat="1">
-      <c r="A80" s="12"/>
+      <c r="A80" s="114"/>
       <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
+      <c r="C80" s="116"/>
       <c r="D80" s="13"/>
       <c r="E80" s="13"/>
       <c r="F80" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G80" s="13" t="str">
@@ -4926,7 +5169,7 @@
         <v/>
       </c>
       <c r="H80" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I80" s="13" t="str">
@@ -4937,13 +5180,13 @@
       <c r="K80" s="14"/>
     </row>
     <row r="81" spans="1:11" s="11" customFormat="1">
-      <c r="A81" s="12"/>
+      <c r="A81" s="114"/>
       <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
+      <c r="C81" s="116"/>
       <c r="D81" s="13"/>
       <c r="E81" s="13"/>
       <c r="F81" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G81" s="13" t="str">
@@ -4951,7 +5194,7 @@
         <v/>
       </c>
       <c r="H81" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I81" s="13" t="str">
@@ -4962,13 +5205,13 @@
       <c r="K81" s="14"/>
     </row>
     <row r="82" spans="1:11" s="11" customFormat="1">
-      <c r="A82" s="12"/>
+      <c r="A82" s="114"/>
       <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
+      <c r="C82" s="116"/>
       <c r="D82" s="13"/>
       <c r="E82" s="13"/>
       <c r="F82" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G82" s="13" t="str">
@@ -4976,7 +5219,7 @@
         <v/>
       </c>
       <c r="H82" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I82" s="13" t="str">
@@ -4987,13 +5230,13 @@
       <c r="K82" s="14"/>
     </row>
     <row r="83" spans="1:11" s="11" customFormat="1">
-      <c r="A83" s="12"/>
+      <c r="A83" s="114"/>
       <c r="B83" s="12"/>
-      <c r="C83" s="12"/>
+      <c r="C83" s="116"/>
       <c r="D83" s="13"/>
       <c r="E83" s="13"/>
       <c r="F83" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G83" s="13" t="str">
@@ -5001,7 +5244,7 @@
         <v/>
       </c>
       <c r="H83" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I83" s="13" t="str">
@@ -5012,13 +5255,13 @@
       <c r="K83" s="14"/>
     </row>
     <row r="84" spans="1:11" s="11" customFormat="1">
-      <c r="A84" s="12"/>
+      <c r="A84" s="114"/>
       <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
+      <c r="C84" s="116"/>
       <c r="D84" s="13"/>
       <c r="E84" s="13"/>
       <c r="F84" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G84" s="13" t="str">
@@ -5026,7 +5269,7 @@
         <v/>
       </c>
       <c r="H84" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I84" s="13" t="str">
@@ -5037,13 +5280,13 @@
       <c r="K84" s="14"/>
     </row>
     <row r="85" spans="1:11" s="11" customFormat="1">
-      <c r="A85" s="12"/>
+      <c r="A85" s="114"/>
       <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
+      <c r="C85" s="116"/>
       <c r="D85" s="13"/>
       <c r="E85" s="13"/>
       <c r="F85" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G85" s="13" t="str">
@@ -5051,7 +5294,7 @@
         <v/>
       </c>
       <c r="H85" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I85" s="13" t="str">
@@ -5062,13 +5305,13 @@
       <c r="K85" s="14"/>
     </row>
     <row r="86" spans="1:11" s="11" customFormat="1">
-      <c r="A86" s="12"/>
+      <c r="A86" s="114"/>
       <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
+      <c r="C86" s="116"/>
       <c r="D86" s="13"/>
       <c r="E86" s="13"/>
       <c r="F86" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F86:F119" si="2">IF(OR(B86&lt;&gt;"",J86&lt;&gt;""),CONCATENATE($C$7,"_",$A86,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I86="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G86" s="13" t="str">
@@ -5076,7 +5319,7 @@
         <v/>
       </c>
       <c r="H86" s="13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="H86:H119" si="3">IF(AND(I86&lt;&gt;"",I86&lt;&gt;0),IF(OR(B86&lt;&gt;"",J86&lt;&gt;""),CONCATENATE($C$7,"_",$A86,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I86" s="13" t="str">
@@ -5087,9 +5330,9 @@
       <c r="K86" s="14"/>
     </row>
     <row r="87" spans="1:11" s="11" customFormat="1">
-      <c r="A87" s="12"/>
+      <c r="A87" s="114"/>
       <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
+      <c r="C87" s="116"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
       <c r="F87" s="13" t="str">
@@ -5112,9 +5355,9 @@
       <c r="K87" s="14"/>
     </row>
     <row r="88" spans="1:11" s="11" customFormat="1">
-      <c r="A88" s="12"/>
+      <c r="A88" s="114"/>
       <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
+      <c r="C88" s="116"/>
       <c r="D88" s="13"/>
       <c r="E88" s="13"/>
       <c r="F88" s="13" t="str">
@@ -5137,9 +5380,9 @@
       <c r="K88" s="14"/>
     </row>
     <row r="89" spans="1:11" s="11" customFormat="1">
-      <c r="A89" s="12"/>
+      <c r="A89" s="114"/>
       <c r="B89" s="12"/>
-      <c r="C89" s="12"/>
+      <c r="C89" s="116"/>
       <c r="D89" s="13"/>
       <c r="E89" s="13"/>
       <c r="F89" s="13" t="str">
@@ -5162,9 +5405,9 @@
       <c r="K89" s="14"/>
     </row>
     <row r="90" spans="1:11" s="11" customFormat="1">
-      <c r="A90" s="12"/>
+      <c r="A90" s="114"/>
       <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
+      <c r="C90" s="116"/>
       <c r="D90" s="13"/>
       <c r="E90" s="13"/>
       <c r="F90" s="13" t="str">
@@ -5187,9 +5430,9 @@
       <c r="K90" s="14"/>
     </row>
     <row r="91" spans="1:11" s="11" customFormat="1">
-      <c r="A91" s="12"/>
+      <c r="A91" s="114"/>
       <c r="B91" s="12"/>
-      <c r="C91" s="12"/>
+      <c r="C91" s="116"/>
       <c r="D91" s="13"/>
       <c r="E91" s="13"/>
       <c r="F91" s="13" t="str">
@@ -5635,6 +5878,281 @@
       </c>
       <c r="J108" s="13"/>
       <c r="K108" s="14"/>
+    </row>
+    <row r="109" spans="1:11" s="11" customFormat="1">
+      <c r="A109" s="12"/>
+      <c r="B109" s="12"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G109" s="13" t="str">
+        <f>IF(F109&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H109" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I109" s="13" t="str">
+        <f>IF(OR(B109&lt;&gt;"",J109&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J109" s="13"/>
+      <c r="K109" s="14"/>
+    </row>
+    <row r="110" spans="1:11" s="11" customFormat="1">
+      <c r="A110" s="12"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G110" s="13" t="str">
+        <f>IF(F110&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H110" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I110" s="13" t="str">
+        <f>IF(OR(B110&lt;&gt;"",J110&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J110" s="13"/>
+      <c r="K110" s="14"/>
+    </row>
+    <row r="111" spans="1:11" s="11" customFormat="1">
+      <c r="A111" s="12"/>
+      <c r="B111" s="12"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G111" s="13" t="str">
+        <f>IF(F111&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H111" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I111" s="13" t="str">
+        <f>IF(OR(B111&lt;&gt;"",J111&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J111" s="13"/>
+      <c r="K111" s="14"/>
+    </row>
+    <row r="112" spans="1:11" s="11" customFormat="1">
+      <c r="A112" s="12"/>
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G112" s="13" t="str">
+        <f>IF(F112&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H112" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I112" s="13" t="str">
+        <f>IF(OR(B112&lt;&gt;"",J112&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J112" s="13"/>
+      <c r="K112" s="14"/>
+    </row>
+    <row r="113" spans="1:11" s="11" customFormat="1">
+      <c r="A113" s="12"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G113" s="13" t="str">
+        <f>IF(F113&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H113" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I113" s="13" t="str">
+        <f>IF(OR(B113&lt;&gt;"",J113&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J113" s="13"/>
+      <c r="K113" s="14"/>
+    </row>
+    <row r="114" spans="1:11" s="11" customFormat="1">
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G114" s="13" t="str">
+        <f>IF(F114&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H114" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I114" s="13" t="str">
+        <f>IF(OR(B114&lt;&gt;"",J114&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J114" s="13"/>
+      <c r="K114" s="14"/>
+    </row>
+    <row r="115" spans="1:11" s="11" customFormat="1">
+      <c r="A115" s="12"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G115" s="13" t="str">
+        <f>IF(F115&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H115" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I115" s="13" t="str">
+        <f>IF(OR(B115&lt;&gt;"",J115&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J115" s="13"/>
+      <c r="K115" s="14"/>
+    </row>
+    <row r="116" spans="1:11" s="11" customFormat="1">
+      <c r="A116" s="12"/>
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G116" s="13" t="str">
+        <f>IF(F116&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H116" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I116" s="13" t="str">
+        <f>IF(OR(B116&lt;&gt;"",J116&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J116" s="13"/>
+      <c r="K116" s="14"/>
+    </row>
+    <row r="117" spans="1:11" s="11" customFormat="1">
+      <c r="A117" s="12"/>
+      <c r="B117" s="12"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G117" s="13" t="str">
+        <f>IF(F117&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H117" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I117" s="13" t="str">
+        <f>IF(OR(B117&lt;&gt;"",J117&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J117" s="13"/>
+      <c r="K117" s="14"/>
+    </row>
+    <row r="118" spans="1:11" s="11" customFormat="1">
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G118" s="13" t="str">
+        <f>IF(F118&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H118" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I118" s="13" t="str">
+        <f>IF(OR(B118&lt;&gt;"",J118&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J118" s="13"/>
+      <c r="K118" s="14"/>
+    </row>
+    <row r="119" spans="1:11" s="11" customFormat="1">
+      <c r="A119" s="12"/>
+      <c r="B119" s="12"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G119" s="13" t="str">
+        <f>IF(F119&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
+        <v/>
+      </c>
+      <c r="H119" s="13" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I119" s="13" t="str">
+        <f>IF(OR(B119&lt;&gt;"",J119&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <v/>
+      </c>
+      <c r="J119" s="13"/>
+      <c r="K119" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5660,10 +6178,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E108">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E14 E16:E119">
       <formula1>"Vertical,Horizontal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D108">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D14 D16:D119">
       <formula1>"Ilustración,Fotografía"</formula1>
     </dataValidation>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:G3">
@@ -5685,12 +6203,15 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1" display="http://www.google.com.co/imgres?imgurl=http://historia1imagen.files.wordpress.com/2013/06/guerra-fria.jpg&amp;imgrefurl=http://historia1imagen.cl/guerra-fria/&amp;h=476&amp;w=544&amp;tbnid=-xBntLZd6KTDXM:&amp;zoom=1&amp;docid=J2VCeC8o2YmSvM&amp;ei=QFDlVLqlLYSnNpS7grAL&amp;tbm=isch&amp;ved=0C"/>
-    <hyperlink ref="B14" r:id="rId2" display="http://www.google.com.co/imgres?imgurl=http://www.esquerda.net/sites/default/files/mapa_de_la_urss_0.jpg&amp;imgrefurl=http://www.esquerda.net/artigos/270&amp;h=542&amp;w=829&amp;tbnid=ANFTAeHdhQE2DM:&amp;zoom=1&amp;docid=zCnmnzvwHI4MyM&amp;ei=gkvlVJu8MomUNriXg6gK&amp;tbm=isch&amp;ved=0CBwQM"/>
-    <hyperlink ref="B21" r:id="rId3"/>
-    <hyperlink ref="B31" r:id="rId4"/>
+    <hyperlink ref="B22" r:id="rId2" display="http://www.google.com.co/imgres?imgurl=http://www.esquerda.net/sites/default/files/mapa_de_la_urss_0.jpg&amp;imgrefurl=http://www.esquerda.net/artigos/270&amp;h=542&amp;w=829&amp;tbnid=ANFTAeHdhQE2DM:&amp;zoom=1&amp;docid=zCnmnzvwHI4MyM&amp;ei=gkvlVJu8MomUNriXg6gK&amp;tbm=isch&amp;ved=0CBwQM"/>
+    <hyperlink ref="B31" r:id="rId3"/>
+    <hyperlink ref="B42" r:id="rId4"/>
+    <hyperlink ref="B11"/>
+    <hyperlink ref="B13" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId7"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5720,25 +6241,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="104"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="99"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
       <c r="A2" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="41"/>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="107"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="102"/>
       <c r="F2" s="42"/>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -5746,11 +6267,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="41"/>
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="112"/>
-      <c r="E3" s="113"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108"/>
       <c r="F3" s="42"/>
       <c r="H3" s="32" t="s">
         <v>18</v>
@@ -5801,11 +6322,11 @@
       <c r="C5" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="114" t="str">
+      <c r="D5" s="109" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="115"/>
+      <c r="E5" s="110"/>
       <c r="F5" s="42"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
@@ -5850,12 +6371,12 @@
       <c r="C7" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="100" t="str">
+      <c r="D7" s="95" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="100"/>
-      <c r="F7" s="101"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="96"/>
       <c r="H7" s="32" t="s">
         <v>24</v>
       </c>
@@ -5949,14 +6470,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="103"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="104"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="99"/>
       <c r="I13" s="32" t="s">
         <v>33</v>
       </c>
@@ -5989,12 +6510,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="41"/>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="107"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="101"/>
+      <c r="F15" s="102"/>
       <c r="J15" s="32">
         <v>12</v>
       </c>
@@ -6034,12 +6555,12 @@
       <c r="C17" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="108" t="str">
+      <c r="D17" s="103" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="109"/>
-      <c r="F17" s="110"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="105"/>
       <c r="J17" s="32">
         <v>14</v>
       </c>
@@ -6055,12 +6576,12 @@
       <c r="C18" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="100" t="str">
+      <c r="D18" s="95" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="100"/>
-      <c r="F18" s="101"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="96"/>
       <c r="J18" s="32">
         <v>15</v>
       </c>
@@ -6452,41 +6973,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="111" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="117" t="s">
+      <c r="H1" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="116"/>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
       <c r="H2" s="51" t="s">
         <v>65</v>
       </c>

</xml_diff>